<commit_message>
dang lan can cho hien thi sinh vien len datagidview
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai lieu mon hoc 2024\Lập trình trực quan\Do an thuc hanh cuoi ky\WinForms_Student_Managed_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai lieu mon hoc 2024\Lập trình trực quan\Do an thuc hanh cuoi ky\WinForms_Student_Managed_app\WinForms_Student_Managed_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05E3D5E-8227-416C-9816-402C1832790C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2A41CA-B738-4833-9658-6991AAFE75CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FDC90BD-B754-4538-A85D-3172C6D805B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>First Name</t>
   </si>
@@ -47,12 +50,12 @@
     <t>Birth Date</t>
   </si>
   <si>
+    <t>Gender</t>
+  </si>
+  <si>
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -90,13 +93,149 @@
   </si>
   <si>
     <t>Bang Coc, Thailand</t>
+  </si>
+  <si>
+    <t>Dang</t>
+  </si>
+  <si>
+    <t>Ngoc Truong Giang</t>
+  </si>
+  <si>
+    <t>3/27/1998</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>Ninh Thuận</t>
+  </si>
+  <si>
+    <t>System.IO.MemoryStream</t>
+  </si>
+  <si>
+    <t>Ngoc Lam</t>
+  </si>
+  <si>
+    <t>1/1/2000</t>
+  </si>
+  <si>
+    <t>1589</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>1/27/1996</t>
+  </si>
+  <si>
+    <t>84956</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>C:\Users\lamda\Pictures\Camera Roll\277100103_263810875962346_2995588130068982526_n.jpg</t>
+  </si>
+  <si>
+    <t>Donale</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>11/27/1975</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>1235</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>C:\Users\lamda\Pictures\Camera Roll\260217298_181205270889574_1606603586922431335_n.jpg</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Hilton</t>
+  </si>
+  <si>
+    <t>3/27/2002</t>
+  </si>
+  <si>
+    <t>1256</t>
+  </si>
+  <si>
+    <t>Washinton</t>
+  </si>
+  <si>
+    <t>C:\Users\lamda\Pictures\Camera Roll\277227889_263810759295691_7379173921303819637_n.jpg</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>fxbxb</t>
+  </si>
+  <si>
+    <t>7/1/1998</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>sfe</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Cso</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>59852</t>
+  </si>
+  <si>
+    <t>Gdavina</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Cao</t>
+  </si>
+  <si>
+    <t>Thanh Tinh</t>
+  </si>
+  <si>
+    <t>7/27/1993</t>
+  </si>
+  <si>
+    <t>1928</t>
+  </si>
+  <si>
+    <t>Dong Da, Ha Noi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,9 +264,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -462,106 +603,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F3526-1F51-4460-9234-8F632CC54DCA}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1" style="2"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1" style="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2">
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
         <v>35584</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0">
         <v>11111111</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34739</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0">
+        <v>22222222</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>35921</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>34739</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>22222222</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>35921</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
+      <c r="F4" s="0">
         <v>33333333</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
+      <c r="G4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
da sua duoc sinh vien bang cach click vao cell trong list sinh vien va cap nhat vao excel
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai lieu mon hoc 2024\Lập trình trực quan\Do an thuc hanh cuoi ky\WinForms_Student_Managed_app\WinForms_Student_Managed_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC44EDB-E05F-48B1-87B3-54E176AF405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2456552-2923-4565-B38B-0F8C18595A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FDC90BD-B754-4538-A85D-3172C6D805B0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Birth Date</t>
+    <t>BirthDay</t>
   </si>
   <si>
     <t>Gender</t>
@@ -56,49 +56,103 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Address</t>
+    <t xml:space="preserve">Address </t>
   </si>
   <si>
     <t>Picture</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truong </t>
-  </si>
-  <si>
-    <t>Giang</t>
-  </si>
-  <si>
-    <t>7/26/1985</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Dang</t>
+  </si>
+  <si>
+    <t>Ngoc Truong Giang</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>489125</t>
-  </si>
-  <si>
-    <t>MelBourne</t>
-  </si>
-  <si>
-    <t>C:\Users\lamda\Pictures\Camera Roll\277100103_263810875962346_2995588130068982526_n.jpg</t>
+    <t>849242</t>
+  </si>
+  <si>
+    <t>Ninh Thuan, Viet Nam</t>
+  </si>
+  <si>
+    <t>D:\UngDungGiangTaiXuong\image.jpg</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Nhat Huy</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Minh Dat</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>157</t>
-  </si>
-  <si>
-    <t>gfsg</t>
-  </si>
-  <si>
-    <t>C:\Users\lamda\Pictures\Camera Roll\260217298_181205270889574_1606603586922431335_n.jpg</t>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Putin</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Putin.jpeg</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>Can Binh</t>
+  </si>
+  <si>
+    <t>2399</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>3025</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\donald-trump.jpg</t>
   </si>
 </sst>
 </file>
@@ -473,22 +527,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F3526-1F51-4460-9234-8F632CC54DCA}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1" style="1"/>
     <col min="2" max="2" width="12.44140625" customWidth="1" style="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1" style="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1" style="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1" style="2"/>
     <col min="5" max="5" width="8.88671875" customWidth="1" style="1"/>
     <col min="6" max="6" width="18.109375" customWidth="1" style="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1" style="1"/>
-    <col min="8" max="8" width="25.109375" customWidth="1" style="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1" style="1"/>
+    <col min="8" max="8" width="35.77734375" customWidth="1" style="1"/>
     <col min="9" max="9" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -528,46 +582,150 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2">
+        <v>38052</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="2">
+        <v>38417</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
+        <v>37044</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2">
-        <v>37253</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2">
+        <v>22286.905996087964</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20459.905996087964</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2">
+        <v>19303.905996087964</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
da xoa duoc thong tin hoc sinh duoc chon trong datagridview bang cach nhan nut remove
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -83,22 +83,16 @@
     <t>D:\UngDungGiangTaiXuong\image.jpg</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Nhat Huy</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Minh Dat</t>
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Nguyen</t>
-  </si>
-  <si>
-    <t>Minh Dat</t>
   </si>
   <si>
     <t>4</t>
@@ -527,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F3526-1F51-4460-9234-8F632CC54DCA}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -603,16 +597,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>38417</v>
+        <v>37044</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
@@ -626,106 +620,80 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
-        <v>37044</v>
+        <v>22286.905996087964</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2">
-        <v>22286.905996087964</v>
+        <v>20459.905996087964</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
-        <v>20459.905996087964</v>
+        <v>19303.905996087964</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="2">
-        <v>19303.905996087964</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
da lam khi click vao form edit/ remove se nhap ma so sv roi nhan nut find se hien thi thong tin sinh vien do, co the dung nut edit va remove de xoa va sua
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -71,37 +71,37 @@
     <t>Ngoc Truong Giang</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>849242</t>
+  </si>
+  <si>
+    <t>Ninh Thuan, Viet Nam</t>
+  </si>
+  <si>
+    <t>D:\UngDungGiangTaiXuong\image.jpg</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Hieu Khanh</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Putin</t>
+  </si>
+  <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>849242</t>
-  </si>
-  <si>
-    <t>Ninh Thuan, Viet Nam</t>
-  </si>
-  <si>
-    <t>D:\UngDungGiangTaiXuong\image.jpg</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Nguyen</t>
-  </si>
-  <si>
-    <t>Minh Dat</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Vladimir</t>
-  </si>
-  <si>
-    <t>Putin</t>
   </si>
   <si>
     <t>1500</t>
@@ -577,7 +577,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>38052</v>
+        <v>37293</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -606,7 +606,7 @@
         <v>37044</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
@@ -620,19 +620,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="2">
         <v>22286.905996087964</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -658,7 +658,7 @@
         <v>20459.905996087964</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>28</v>
@@ -684,7 +684,7 @@
         <v>19303.905996087964</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
da lam statistics se thong ke tong so sinh vien va ty le nam nu
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -92,7 +92,46 @@
     <t>Hieu Khanh</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>Can Binh</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2399</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>3025</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\donald-trump.jpg</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Vladimir</t>
@@ -101,52 +140,10 @@
     <t>Putin</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
     <t>Russia</t>
   </si>
   <si>
     <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Putin.jpeg</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Tap</t>
-  </si>
-  <si>
-    <t>Can Binh</t>
-  </si>
-  <si>
-    <t>2399</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Donald</t>
-  </si>
-  <si>
-    <t>Trump</t>
-  </si>
-  <si>
-    <t>3025</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\donald-trump.jpg</t>
   </si>
 </sst>
 </file>
@@ -629,7 +626,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="2">
-        <v>22286.905996087964</v>
+        <v>20459.905996087964</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
@@ -655,10 +652,10 @@
         <v>27</v>
       </c>
       <c r="D5" s="2">
-        <v>20459.905996087964</v>
+        <v>19303.905996087964</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>28</v>
@@ -681,19 +678,19 @@
         <v>33</v>
       </c>
       <c r="D6" s="2">
-        <v>19303.905996087964</v>
+        <v>26851.6518209375</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
da lam form manage studens, co the dung search de loc sinh vien can tim va thuc hien them, xoa, sua sinh vien do, nhan reset de xem lai danh sach sinh vien trong excel sau khi thuc hien cac thao tac tren
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai lieu mon hoc 2024\Lập trình trực quan\Do an thuc hanh cuoi ky\WinForms_Student_Managed_app\WinForms_Student_Managed_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2456552-2923-4565-B38B-0F8C18595A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96DB6E5-1749-4647-B433-2FEEE9363C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FDC90BD-B754-4538-A85D-3172C6D805B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trang_tính2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -83,67 +84,64 @@
     <t>D:\UngDungGiangTaiXuong\image.jpg</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Tap</t>
+  </si>
+  <si>
+    <t>Can Binh</t>
+  </si>
+  <si>
+    <t>2399</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Nguyen</t>
-  </si>
-  <si>
-    <t>Hieu Khanh</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Tap</t>
-  </si>
-  <si>
-    <t>Can Binh</t>
+    <t>Duong</t>
+  </si>
+  <si>
+    <t>Yen Nhi</t>
+  </si>
+  <si>
+    <t>1579</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Putin</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>2399</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Donald</t>
-  </si>
-  <si>
-    <t>Trump</t>
-  </si>
-  <si>
-    <t>3025</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\donald-trump.jpg</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Vladimir</t>
-  </si>
-  <si>
-    <t>Putin</t>
+    <t>1933</t>
   </si>
   <si>
     <t>Russia</t>
   </si>
   <si>
     <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Putin.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng sinh viên </t>
+  </si>
+  <si>
+    <t>Tỉ lệ nam %</t>
+  </si>
+  <si>
+    <t>Tỉ lệ nữ %</t>
   </si>
 </sst>
 </file>
@@ -518,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F3526-1F51-4460-9234-8F632CC54DCA}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,45 +598,45 @@
         <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>37044</v>
+        <v>20459.905996087964</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2">
+        <v>36957.63684953703</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="2">
-        <v>20459.905996087964</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -652,45 +650,19 @@
         <v>27</v>
       </c>
       <c r="D5" s="2">
-        <v>19303.905996087964</v>
+        <v>20827.638431944444</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2">
-        <v>26851.6518209375</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -698,4 +670,47 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48C59AD-BF55-437A-B7AB-B00403A8328F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
luu y khi edit sau khi search thi khong duoc sua ID vi nut edit tim dong de sua tren excel dua vao ID
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -66,25 +66,25 @@
     <t>1</t>
   </si>
   <si>
-    <t>Dang</t>
-  </si>
-  <si>
-    <t>Ngoc Truong Giang</t>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Rose</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>849242</t>
-  </si>
-  <si>
-    <t>Ninh Thuan, Viet Nam</t>
-  </si>
-  <si>
-    <t>D:\UngDungGiangTaiXuong\image.jpg</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Rose.jpeg</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Tap</t>
@@ -93,10 +93,13 @@
     <t>Can Binh</t>
   </si>
   <si>
-    <t>2399</t>
-  </si>
-  <si>
-    <t>China</t>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Beijing</t>
   </si>
   <si>
     <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
@@ -105,34 +108,34 @@
     <t>3</t>
   </si>
   <si>
-    <t>Duong</t>
-  </si>
-  <si>
-    <t>Yen Nhi</t>
-  </si>
-  <si>
-    <t>1579</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Vladimir</t>
-  </si>
-  <si>
-    <t>Putin</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>1933</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Putin.jpeg</t>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Tieu Dao</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>Quang Dong</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Ma Tieu Dao.jpeg</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Van Thuong</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>Tham Quyen</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Bi Bi Dong.jpeg</t>
   </si>
   <si>
     <t xml:space="preserve">Tổng sinh viên </t>
@@ -572,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>37293</v>
+        <v>36501.94482556713</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -598,71 +601,71 @@
         <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>20459.905996087964</v>
+        <v>18239.963888958333</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2">
-        <v>36957.63684953703</v>
+        <v>34706.9646059838</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2">
-        <v>20827.638431944444</v>
+        <v>27599.966736493054</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -689,24 +692,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mini project is completed
</commit_message>
<xml_diff>
--- a/data_SinhVien.xlsx
+++ b/data_SinhVien.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -66,73 +66,58 @@
     <t>1</t>
   </si>
   <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Rose</t>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Putin</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>12589</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Putin.jpeg</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Tieu Dao</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>Korea</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Rose.jpeg</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Tap</t>
-  </si>
-  <si>
-    <t>Can Binh</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>Beijing</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Tap can binh.jpeg</t>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Quang Chau</t>
+  </si>
+  <si>
+    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Ma Tieu Dao.jpeg</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>Tieu Dao</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>Quang Dong</t>
-  </si>
-  <si>
-    <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Ma Tieu Dao.jpeg</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Van Thuong</t>
-  </si>
-  <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>Tham Quyen</t>
+    <t>Bi Bi</t>
+  </si>
+  <si>
+    <t>Dong</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>Quang Nam</t>
   </si>
   <si>
     <t>D:\Tai lieu mon hoc 2024\Lập trình trực quan\Bi Bi Dong.jpeg</t>
@@ -519,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F3526-1F51-4460-9234-8F632CC54DCA}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -575,7 +560,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>36501.94482556713</v>
+        <v>36244.42661986111</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -601,7 +586,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>18239.963888958333</v>
+        <v>31237.429842002315</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -627,10 +612,10 @@
         <v>24</v>
       </c>
       <c r="D4" s="2">
-        <v>34706.9646059838</v>
+        <v>-16092.430743344907</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>25</v>
@@ -640,32 +625,6 @@
       </c>
       <c r="H4" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2">
-        <v>27599.966736493054</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -692,13 +651,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -706,10 +665,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>